<commit_message>
Test commit XLSX via Apps Script
</commit_message>
<xml_diff>
--- a/stest_time-sheet-wssoa-2025.xlsx
+++ b/stest_time-sheet-wssoa-2025.xlsx
@@ -22,7 +22,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="H9">
+    <comment authorId="0" ref="H5">
       <text>
         <t xml:space="preserve">======
 ID#AAAAhHKzbRo
@@ -30,7 +30,7 @@
 Enter your name here. It will automatically be copied to all time sheets.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H10">
+    <comment authorId="0" ref="H6">
       <text>
         <t xml:space="preserve">======
 ID#AAAAhHKzbR4
@@ -38,7 +38,7 @@
 Enter your title/function here. It will automatically be copied to all the time sheets.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N11">
+    <comment authorId="0" ref="N7">
       <text>
         <t xml:space="preserve">======
 ID#AAAAhHKzbRg
@@ -46,7 +46,7 @@
 Indicate which department you belong to</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H13">
+    <comment authorId="0" ref="H9">
       <text>
         <t xml:space="preserve">======
 ID#AAAAhHKzbRs
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="68">
   <si>
     <t>Time sheets for WS&amp;SOA project</t>
   </si>
@@ -118,25 +118,10 @@
     <t>Service-Booking-System</t>
   </si>
   <si>
-    <t>Title project 2:</t>
-  </si>
-  <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>Title project 3:</t>
-  </si>
-  <si>
-    <t>Title project 4:</t>
-  </si>
-  <si>
-    <t>Contact No:</t>
-  </si>
-  <si>
     <t>Person responsible:</t>
   </si>
   <si>
-    <t>Your Name</t>
+    <t>Malhar Prajapati</t>
   </si>
   <si>
     <t>Title/Designation:</t>
@@ -154,7 +139,7 @@
     <t>Person In-Charge</t>
   </si>
   <si>
-    <t>Name of Your TA / Supervisor</t>
+    <t>Dr Jayprakash Lalchandani</t>
   </si>
   <si>
     <t>Title:</t>
@@ -281,6 +266,9 @@
     <t>Total 
 Prod. 
 Hours</t>
+  </si>
+  <si>
+    <t>Brainstorming</t>
   </si>
   <si>
     <t>Total</t>
@@ -749,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -985,13 +973,16 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="25" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="26" fillId="0" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="24" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -8399,7 +8390,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="14"/>
@@ -8426,7 +8417,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -8443,7 +8434,7 @@
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -8451,15 +8442,15 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
+      <c r="H7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="W7" s="8"/>
@@ -8469,7 +8460,7 @@
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -8477,8 +8468,8 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="13" t="s">
-        <v>17</v>
+      <c r="H8" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -8495,7 +8486,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -8504,7 +8495,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
       <c r="H9" s="13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -8520,24 +8511,20 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="W10" s="8"/>
@@ -8545,193 +8532,235 @@
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
+    <row r="11" ht="24.75" customHeight="1">
+      <c r="A11" s="17" t="str">
+        <f>H5</f>
+        <v>Malhar Prajapati</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19" t="str">
+        <f>H4</f>
+        <v>Service-Booking-System</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
+      <c r="X12" s="24"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="13" t="s">
+    <row r="13" ht="25.5" customHeight="1">
+      <c r="A13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27">
+        <v>45866.0</v>
+      </c>
+      <c r="D13" s="27">
+        <v>45870.0</v>
+      </c>
+      <c r="E13" s="28">
+        <v>45901.0</v>
+      </c>
+      <c r="F13" s="28">
+        <v>45931.0</v>
+      </c>
+      <c r="G13" s="28">
+        <v>45962.0</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="36">
+        <f>4-'Jul-25'!E14</f>
+        <v>4</v>
+      </c>
+      <c r="D15" s="36">
+        <f>31-'Aug-25'!E41</f>
+        <v>31</v>
+      </c>
+      <c r="E15" s="36">
+        <f>30-'Sep-25'!E40</f>
         <v>30</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-    </row>
-    <row r="15" ht="24.75" customHeight="1">
-      <c r="A15" s="17" t="str">
-        <f>H9</f>
-        <v>Your Name</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="str">
-        <f>H4</f>
-        <v>Service-Booking-System</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="23"/>
+      <c r="F15" s="36">
+        <f>31-'Oct-25'!E41</f>
+        <v>31</v>
+      </c>
+      <c r="G15" s="36">
+        <f>20-'Nov-25'!E30</f>
+        <v>20</v>
+      </c>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34"/>
       <c r="X15" s="22"/>
       <c r="Y15" s="22"/>
       <c r="Z15" s="22"/>
     </row>
     <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="24"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" ht="25.5" customHeight="1">
-      <c r="A17" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27">
-        <v>45866.0</v>
-      </c>
-      <c r="D17" s="27">
-        <v>45870.0</v>
-      </c>
-      <c r="E17" s="28">
-        <v>45901.0</v>
-      </c>
-      <c r="F17" s="28">
-        <v>45931.0</v>
-      </c>
-      <c r="G17" s="28">
-        <v>45962.0</v>
-      </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="41">
+        <f>'Jul-25'!E14</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="41">
+        <f>'Aug-25'!E41</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="36">
+        <f>'Sep-25'!E40</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="36">
+        <f>'Oct-25'!E41</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="36">
+        <f>'Nov-25'!E30</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="34"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="42"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="44"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
@@ -8745,37 +8774,37 @@
       <c r="T18" s="34"/>
       <c r="U18" s="34"/>
       <c r="V18" s="34"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22"/>
-      <c r="Z18" s="22"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="35" t="s">
-        <v>32</v>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="45" t="s">
+        <v>29</v>
       </c>
       <c r="B19" s="18"/>
-      <c r="C19" s="36">
-        <f>4-'Jul-25'!E14</f>
-        <v>4</v>
-      </c>
-      <c r="D19" s="36">
-        <f>31-'Aug-25'!E41</f>
-        <v>31</v>
-      </c>
-      <c r="E19" s="36">
-        <f>30-'Sep-25'!E40</f>
-        <v>30</v>
-      </c>
-      <c r="F19" s="36">
-        <f>31-'Oct-25'!E41</f>
-        <v>31</v>
-      </c>
-      <c r="G19" s="36">
-        <f>20-'Nov-25'!E30</f>
-        <v>20</v>
+      <c r="C19" s="46">
+        <f>'Jul-25'!F14</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="46">
+        <f>'Aug-25'!F41</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="46">
+        <f>'Sep-25'!F40</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="46">
+        <f>'Oct-25'!F41</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="46">
+        <f>'Nov-25'!F30</f>
+        <v>0</v>
       </c>
       <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
+      <c r="I19" s="47"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
@@ -8793,356 +8822,311 @@
       <c r="Y19" s="22"/>
       <c r="Z19" s="22"/>
     </row>
-    <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="W20" s="48"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="41">
-        <f>'Jul-25'!E14</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="41">
-        <f>'Aug-25'!E41</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="36">
-        <f>'Sep-25'!E40</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="36">
-        <f>'Oct-25'!E41</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="36">
-        <f>'Nov-25'!E30</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="34"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="W21" s="48"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="42"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="34"/>
+      <c r="A22" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="52"/>
+      <c r="T22" s="51"/>
+      <c r="W22" s="48"/>
       <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="46">
-        <f>'Jul-25'!F14</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="46">
-        <f>'Aug-25'!F41</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="46">
-        <f>'Sep-25'!F40</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="46">
-        <f>'Oct-25'!F41</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="46">
-        <f>'Nov-25'!F30</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="34"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="22"/>
-      <c r="Z23" s="22"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="51"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
       <c r="J24" s="48"/>
       <c r="K24" s="48"/>
       <c r="L24" s="48"/>
       <c r="M24" s="48"/>
       <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="48"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="51"/>
       <c r="W24" s="48"/>
       <c r="X24" s="8"/>
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="8"/>
+      <c r="A25" s="8" t="str">
+        <f t="shared" ref="A25:A26" si="1">H5</f>
+        <v>Malhar Prajapati</v>
+      </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="str">
+        <f t="shared" ref="G25:G26" si="2">H8</f>
+        <v>Dr Jayprakash Lalchandani</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
       <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="48"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
       <c r="W25" s="48"/>
       <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
+      <c r="A26" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Team Member</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Dr/Prof</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
       <c r="N26" s="48"/>
-      <c r="O26" s="50"/>
+      <c r="O26" s="51"/>
       <c r="P26" s="51"/>
       <c r="Q26" s="52"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="52"/>
-      <c r="T26" s="51"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="51"/>
       <c r="W26" s="48"/>
       <c r="X26" s="8"/>
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="48"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
       <c r="N27" s="48"/>
       <c r="O27" s="51"/>
       <c r="P27" s="51"/>
-      <c r="Q27" s="52"/>
       <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="51"/>
       <c r="W27" s="48"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
+      <c r="A28" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="56"/>
+      <c r="N28" s="8"/>
       <c r="O28" s="51"/>
       <c r="P28" s="51"/>
       <c r="Q28" s="52"/>
       <c r="R28" s="51"/>
-      <c r="W28" s="48"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="51"/>
+      <c r="W28" s="8"/>
       <c r="X28" s="8"/>
       <c r="Y28" s="8"/>
       <c r="Z28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="8" t="str">
-        <f t="shared" ref="A29:A30" si="1">H9</f>
-        <v>Your Name</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8" t="str">
-        <f t="shared" ref="G29:G30" si="2">H12</f>
-        <v>Name of Your TA / Supervisor</v>
-      </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="52"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="W29" s="48"/>
+      <c r="A29" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="60"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="W29" s="8"/>
       <c r="X29" s="8"/>
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Team Member</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Dr/Prof</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="51"/>
-      <c r="W30" s="48"/>
+      <c r="A30" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="59"/>
+      <c r="D30" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="60"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="W30" s="8"/>
       <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="51"/>
-      <c r="W31" s="48"/>
+      <c r="A31" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="60"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="W31" s="8"/>
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="56"/>
+      <c r="A32" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="60"/>
+      <c r="D32" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="58"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
       <c r="N32" s="8"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="51"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
       <c r="W32" s="8"/>
       <c r="X32" s="8"/>
       <c r="Y32" s="8"/>
@@ -9150,21 +9134,29 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="58" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C33" s="59"/>
       <c r="D33" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="60"/>
+        <v>51</v>
+      </c>
+      <c r="E33" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="58"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
       <c r="Y33" s="8"/>
@@ -9172,41 +9164,44 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="58" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C34" s="59"/>
-      <c r="D34" s="61" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="60"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="60"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -9216,20 +9211,12 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="60"/>
-      <c r="D36" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
@@ -9246,20 +9233,12 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -9276,16 +9255,12 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="58"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
@@ -13613,94 +13588,10 @@
       <c r="Y234" s="8"/>
       <c r="Z234" s="8"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="8"/>
-      <c r="B235" s="8"/>
-      <c r="C235" s="8"/>
-      <c r="D235" s="8"/>
-      <c r="E235" s="8"/>
-      <c r="F235" s="8"/>
-      <c r="G235" s="8"/>
-      <c r="H235" s="8"/>
-      <c r="I235" s="8"/>
-      <c r="J235" s="8"/>
-      <c r="K235" s="8"/>
-      <c r="L235" s="8"/>
-      <c r="M235" s="8"/>
-      <c r="N235" s="8"/>
-      <c r="O235" s="8"/>
-      <c r="P235" s="8"/>
-      <c r="W235" s="8"/>
-      <c r="X235" s="8"/>
-      <c r="Y235" s="8"/>
-      <c r="Z235" s="8"/>
-    </row>
-    <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="8"/>
-      <c r="B236" s="8"/>
-      <c r="C236" s="8"/>
-      <c r="D236" s="8"/>
-      <c r="E236" s="8"/>
-      <c r="F236" s="8"/>
-      <c r="G236" s="8"/>
-      <c r="H236" s="8"/>
-      <c r="I236" s="8"/>
-      <c r="J236" s="8"/>
-      <c r="K236" s="8"/>
-      <c r="L236" s="8"/>
-      <c r="M236" s="8"/>
-      <c r="N236" s="8"/>
-      <c r="O236" s="8"/>
-      <c r="P236" s="8"/>
-      <c r="W236" s="8"/>
-      <c r="X236" s="8"/>
-      <c r="Y236" s="8"/>
-      <c r="Z236" s="8"/>
-    </row>
-    <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="8"/>
-      <c r="B237" s="8"/>
-      <c r="C237" s="8"/>
-      <c r="D237" s="8"/>
-      <c r="E237" s="8"/>
-      <c r="F237" s="8"/>
-      <c r="G237" s="8"/>
-      <c r="H237" s="8"/>
-      <c r="I237" s="8"/>
-      <c r="J237" s="8"/>
-      <c r="K237" s="8"/>
-      <c r="L237" s="8"/>
-      <c r="M237" s="8"/>
-      <c r="N237" s="8"/>
-      <c r="O237" s="8"/>
-      <c r="P237" s="8"/>
-      <c r="W237" s="8"/>
-      <c r="X237" s="8"/>
-      <c r="Y237" s="8"/>
-      <c r="Z237" s="8"/>
-    </row>
-    <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="8"/>
-      <c r="B238" s="8"/>
-      <c r="C238" s="8"/>
-      <c r="D238" s="8"/>
-      <c r="E238" s="8"/>
-      <c r="F238" s="8"/>
-      <c r="G238" s="8"/>
-      <c r="H238" s="8"/>
-      <c r="I238" s="8"/>
-      <c r="J238" s="8"/>
-      <c r="K238" s="8"/>
-      <c r="L238" s="8"/>
-      <c r="M238" s="8"/>
-      <c r="N238" s="8"/>
-      <c r="O238" s="8"/>
-      <c r="P238" s="8"/>
-      <c r="W238" s="8"/>
-      <c r="X238" s="8"/>
-      <c r="Y238" s="8"/>
-      <c r="Z238" s="8"/>
-    </row>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
     <row r="239" ht="15.75" customHeight="1"/>
     <row r="240" ht="15.75" customHeight="1"/>
     <row r="241" ht="15.75" customHeight="1"/>
@@ -14459,31 +14350,23 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="15">
     <mergeCell ref="H3:N3"/>
     <mergeCell ref="H4:N4"/>
     <mergeCell ref="H5:N5"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="H6:N6"/>
-    <mergeCell ref="H7:N7"/>
     <mergeCell ref="H8:N8"/>
     <mergeCell ref="H9:N9"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:G14"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -14521,18 +14404,18 @@
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="62"/>
       <c r="E1" s="8"/>
       <c r="F1" s="62"/>
       <c r="G1" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H1" s="63" t="str">
-        <f>Overview!H9</f>
-        <v>Your Name</v>
+        <f>Overview!H5</f>
+        <v>Malhar Prajapati</v>
       </c>
       <c r="K1" s="62"/>
       <c r="L1" s="62"/>
@@ -14548,7 +14431,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="62"/>
       <c r="G2" s="64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" s="65">
         <v>45839.0</v>
@@ -14566,7 +14449,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="62"/>
       <c r="G3" s="64" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="66" t="str">
         <f>Overview!H3</f>
@@ -14593,7 +14476,7 @@
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="70" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>Overview!H4</f>
@@ -14622,19 +14505,19 @@
     <row r="7" ht="33.75" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="72" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
@@ -14653,7 +14536,9 @@
       <c r="B9" s="81">
         <v>28.0</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="82" t="s">
+        <v>65</v>
+      </c>
       <c r="D9" s="83">
         <v>0.0</v>
       </c>
@@ -14670,7 +14555,7 @@
       <c r="B10" s="81">
         <v>29.0</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="83">
         <v>0.0</v>
       </c>
@@ -14687,7 +14572,7 @@
       <c r="B11" s="81">
         <v>30.0</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="83">
         <v>0.0</v>
       </c>
@@ -14704,7 +14589,7 @@
       <c r="B12" s="81">
         <v>31.0</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="83">
         <v>0.0</v>
       </c>
@@ -14718,30 +14603,30 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="85"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
       <c r="F13" s="84"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C14" s="72" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
       </c>
-      <c r="D14" s="88">
+      <c r="D14" s="89">
         <f t="shared" ref="D14:F14" si="2">SUM(D9:D13)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="89">
+      <c r="E14" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F14" s="89">
+      <c r="F14" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -14750,7 +14635,7 @@
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="48"/>
-      <c r="D15" s="90"/>
+      <c r="D15" s="91"/>
       <c r="E15" s="8"/>
       <c r="F15" s="62"/>
       <c r="G15" s="8"/>
@@ -14763,7 +14648,7 @@
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="57"/>
@@ -14779,17 +14664,17 @@
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="8"/>
       <c r="B17" s="58" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D17" s="59"/>
       <c r="E17" s="58" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F17" s="58" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G17" s="60"/>
       <c r="H17" s="62"/>
@@ -14801,68 +14686,68 @@
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="61" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F18" s="58" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G18" s="60"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" s="58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D19" s="59"/>
       <c r="E19" s="60" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G19" s="60"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D20" s="60"/>
       <c r="E20" s="58" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F20" s="58" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G20" s="58"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="8"/>
       <c r="B21" s="58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D21" s="59"/>
       <c r="E21" s="58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G21" s="58"/>
       <c r="H21" s="62"/>
@@ -14874,10 +14759,10 @@
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="58" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="59"/>
       <c r="E22" s="58"/>
@@ -14891,7 +14776,7 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="H23" s="91"/>
+      <c r="H23" s="92"/>
       <c r="I23" s="8"/>
       <c r="J23" s="62"/>
       <c r="K23" s="62"/>
@@ -14900,9 +14785,9 @@
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="8"/>
       <c r="B24" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" s="91"/>
+        <v>67</v>
+      </c>
+      <c r="H24" s="92"/>
       <c r="I24" s="8"/>
       <c r="J24" s="62"/>
       <c r="K24" s="62"/>
@@ -15928,18 +15813,18 @@
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="62"/>
       <c r="E1" s="8"/>
       <c r="F1" s="62"/>
       <c r="G1" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H1" s="63" t="str">
-        <f>Overview!H9</f>
-        <v>Your Name</v>
+        <f>Overview!H5</f>
+        <v>Malhar Prajapati</v>
       </c>
       <c r="K1" s="62"/>
       <c r="L1" s="62"/>
@@ -15955,7 +15840,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="62"/>
       <c r="G2" s="64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" s="65">
         <v>45870.0</v>
@@ -15973,7 +15858,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="62"/>
       <c r="G3" s="64" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="66" t="str">
         <f>Overview!H3</f>
@@ -16000,7 +15885,7 @@
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="70" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>Overview!H4</f>
@@ -16028,26 +15913,26 @@
     </row>
     <row r="7" ht="33.75" customHeight="1">
       <c r="A7" s="22"/>
-      <c r="B7" s="92" t="s">
-        <v>65</v>
+      <c r="B7" s="93" t="s">
+        <v>60</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="22"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="94" t="str">
+      <c r="B8" s="94"/>
+      <c r="C8" s="95" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
       </c>
@@ -16057,10 +15942,10 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="8"/>
-      <c r="B9" s="95">
+      <c r="B9" s="96">
         <v>1.0</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="84">
         <v>0.0</v>
       </c>
@@ -16074,10 +15959,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="8"/>
-      <c r="B10" s="95">
+      <c r="B10" s="96">
         <v>2.0</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="83">
         <v>0.0</v>
       </c>
@@ -16091,10 +15976,10 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="95">
+      <c r="B11" s="96">
         <v>3.0</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="83">
         <v>0.0</v>
       </c>
@@ -16108,10 +15993,10 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="8"/>
-      <c r="B12" s="95">
+      <c r="B12" s="96">
         <v>4.0</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="83">
         <v>0.0</v>
       </c>
@@ -16125,10 +16010,10 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="95">
+      <c r="B13" s="96">
         <v>5.0</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="83">
         <v>0.0</v>
       </c>
@@ -16142,10 +16027,10 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="95">
+      <c r="B14" s="96">
         <v>6.0</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="83">
         <v>0.0</v>
       </c>
@@ -16159,10 +16044,10 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="95">
+      <c r="B15" s="96">
         <v>7.0</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="83">
         <v>0.0</v>
       </c>
@@ -16176,10 +16061,10 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="95">
+      <c r="B16" s="96">
         <v>8.0</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="83">
         <v>0.0</v>
       </c>
@@ -16193,10 +16078,10 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="8"/>
-      <c r="B17" s="95">
+      <c r="B17" s="96">
         <v>9.0</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="83">
         <v>0.0</v>
       </c>
@@ -16210,10 +16095,10 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="8"/>
-      <c r="B18" s="95">
+      <c r="B18" s="96">
         <v>10.0</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="83">
         <v>0.0</v>
       </c>
@@ -16227,10 +16112,10 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="95">
+      <c r="B19" s="96">
         <v>11.0</v>
       </c>
-      <c r="C19" s="82"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="83">
         <v>0.0</v>
       </c>
@@ -16244,10 +16129,10 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="95">
+      <c r="B20" s="96">
         <v>12.0</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="83">
         <v>0.0</v>
       </c>
@@ -16261,10 +16146,10 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="95">
+      <c r="B21" s="96">
         <v>13.0</v>
       </c>
-      <c r="C21" s="82"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="83">
         <v>0.0</v>
       </c>
@@ -16278,10 +16163,10 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="8"/>
-      <c r="B22" s="95">
+      <c r="B22" s="96">
         <v>14.0</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="83">
         <v>0.0</v>
       </c>
@@ -16295,10 +16180,10 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="95">
+      <c r="B23" s="96">
         <v>15.0</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="83">
         <v>0.0</v>
       </c>
@@ -16312,10 +16197,10 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="95">
+      <c r="B24" s="96">
         <v>16.0</v>
       </c>
-      <c r="C24" s="82"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="83">
         <v>0.0</v>
       </c>
@@ -16329,10 +16214,10 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="95">
+      <c r="B25" s="96">
         <v>17.0</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="83">
         <v>0.0</v>
       </c>
@@ -16346,10 +16231,10 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="95">
+      <c r="B26" s="96">
         <v>18.0</v>
       </c>
-      <c r="C26" s="82"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="83">
         <v>0.0</v>
       </c>
@@ -16363,10 +16248,10 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="95">
+      <c r="B27" s="96">
         <v>19.0</v>
       </c>
-      <c r="C27" s="82"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="83">
         <v>0.0</v>
       </c>
@@ -16380,10 +16265,10 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="95">
+      <c r="B28" s="96">
         <v>20.0</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="83">
         <v>0.0</v>
       </c>
@@ -16397,10 +16282,10 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="95">
+      <c r="B29" s="96">
         <v>21.0</v>
       </c>
-      <c r="C29" s="82"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="83">
         <v>0.0</v>
       </c>
@@ -16414,10 +16299,10 @@
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="95">
+      <c r="B30" s="96">
         <v>22.0</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="83">
         <v>0.0</v>
       </c>
@@ -16431,10 +16316,10 @@
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="95">
+      <c r="B31" s="96">
         <v>23.0</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="83">
         <v>0.0</v>
       </c>
@@ -16448,10 +16333,10 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="95">
+      <c r="B32" s="96">
         <v>24.0</v>
       </c>
-      <c r="C32" s="82"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="83">
         <v>0.0</v>
       </c>
@@ -16465,10 +16350,10 @@
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="B33" s="95">
+      <c r="B33" s="96">
         <v>25.0</v>
       </c>
-      <c r="C33" s="82"/>
+      <c r="C33" s="85"/>
       <c r="D33" s="83">
         <v>0.0</v>
       </c>
@@ -16482,10 +16367,10 @@
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="95">
+      <c r="B34" s="96">
         <v>26.0</v>
       </c>
-      <c r="C34" s="82"/>
+      <c r="C34" s="85"/>
       <c r="D34" s="83">
         <v>0.0</v>
       </c>
@@ -16499,10 +16384,10 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="8"/>
-      <c r="B35" s="95">
+      <c r="B35" s="96">
         <v>27.0</v>
       </c>
-      <c r="C35" s="82"/>
+      <c r="C35" s="85"/>
       <c r="D35" s="83">
         <v>0.0</v>
       </c>
@@ -16516,10 +16401,10 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="8"/>
-      <c r="B36" s="95">
+      <c r="B36" s="96">
         <v>28.0</v>
       </c>
-      <c r="C36" s="82"/>
+      <c r="C36" s="85"/>
       <c r="D36" s="83">
         <v>0.0</v>
       </c>
@@ -16533,10 +16418,10 @@
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="8"/>
-      <c r="B37" s="95">
+      <c r="B37" s="96">
         <v>29.0</v>
       </c>
-      <c r="C37" s="82"/>
+      <c r="C37" s="85"/>
       <c r="D37" s="83">
         <v>0.0</v>
       </c>
@@ -16550,10 +16435,10 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="8"/>
-      <c r="B38" s="95">
+      <c r="B38" s="96">
         <v>30.0</v>
       </c>
-      <c r="C38" s="82"/>
+      <c r="C38" s="85"/>
       <c r="D38" s="83">
         <v>0.0</v>
       </c>
@@ -16567,10 +16452,10 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="8"/>
-      <c r="B39" s="95">
+      <c r="B39" s="96">
         <v>31.0</v>
       </c>
-      <c r="C39" s="82"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="83">
         <v>0.0</v>
       </c>
@@ -16584,30 +16469,30 @@
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="8"/>
-      <c r="B40" s="97"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="88"/>
       <c r="F40" s="84"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="22"/>
       <c r="B41" s="72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C41" s="72" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
       </c>
-      <c r="D41" s="88">
+      <c r="D41" s="89">
         <f t="shared" ref="D41:F41" si="2">SUM(D9:D40)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="89">
+      <c r="E41" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F41" s="89">
+      <c r="F41" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -16616,7 +16501,7 @@
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="48"/>
-      <c r="D42" s="90"/>
+      <c r="D42" s="91"/>
       <c r="E42" s="8"/>
       <c r="F42" s="62"/>
       <c r="G42" s="8"/>
@@ -16629,7 +16514,7 @@
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="8"/>
       <c r="B43" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C43" s="56"/>
       <c r="D43" s="57"/>
@@ -16645,17 +16530,17 @@
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="8"/>
       <c r="B44" s="58" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D44" s="59"/>
       <c r="E44" s="58" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F44" s="58" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G44" s="60"/>
       <c r="H44" s="62"/>
@@ -16667,68 +16552,68 @@
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="8"/>
       <c r="B45" s="58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D45" s="59"/>
       <c r="E45" s="61" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F45" s="58" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G45" s="60"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="8"/>
       <c r="B46" s="58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C46" s="58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="60" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F46" s="60" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G46" s="60"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="8"/>
       <c r="B47" s="58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D47" s="60"/>
       <c r="E47" s="58" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F47" s="58" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G47" s="58"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="8"/>
       <c r="B48" s="58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D48" s="59"/>
       <c r="E48" s="58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F48" s="61" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G48" s="58"/>
       <c r="H48" s="62"/>
@@ -16740,10 +16625,10 @@
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="8"/>
       <c r="B49" s="58" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="58"/>
@@ -16757,7 +16642,7 @@
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="8"/>
-      <c r="H50" s="91"/>
+      <c r="H50" s="92"/>
       <c r="I50" s="8"/>
       <c r="J50" s="62"/>
       <c r="K50" s="62"/>
@@ -16766,9 +16651,9 @@
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="8"/>
       <c r="B51" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="H51" s="91"/>
+        <v>67</v>
+      </c>
+      <c r="H51" s="92"/>
       <c r="I51" s="8"/>
       <c r="J51" s="62"/>
       <c r="K51" s="62"/>
@@ -17767,18 +17652,18 @@
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="62"/>
       <c r="E1" s="8"/>
       <c r="F1" s="62"/>
       <c r="G1" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H1" s="63" t="str">
-        <f>Overview!H9</f>
-        <v>Your Name</v>
+        <f>Overview!H5</f>
+        <v>Malhar Prajapati</v>
       </c>
       <c r="K1" s="62"/>
       <c r="L1" s="62"/>
@@ -17794,7 +17679,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="62"/>
       <c r="G2" s="64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" s="65">
         <v>45901.0</v>
@@ -17812,7 +17697,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="62"/>
       <c r="G3" s="64" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="66" t="str">
         <f>Overview!H3</f>
@@ -17839,7 +17724,7 @@
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="70" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>Overview!H4</f>
@@ -17868,24 +17753,24 @@
     <row r="7" ht="33.75" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="72" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="22"/>
-      <c r="B8" s="98"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="77" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
@@ -17896,10 +17781,10 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="8"/>
-      <c r="B9" s="95">
+      <c r="B9" s="96">
         <v>1.0</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="84">
         <v>0.0</v>
       </c>
@@ -17913,10 +17798,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="8"/>
-      <c r="B10" s="95">
+      <c r="B10" s="96">
         <v>2.0</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="83">
         <v>0.0</v>
       </c>
@@ -17930,10 +17815,10 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="95">
+      <c r="B11" s="96">
         <v>3.0</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="83">
         <v>0.0</v>
       </c>
@@ -17947,10 +17832,10 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="8"/>
-      <c r="B12" s="95">
+      <c r="B12" s="96">
         <v>4.0</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="83">
         <v>0.0</v>
       </c>
@@ -17964,10 +17849,10 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="95">
+      <c r="B13" s="96">
         <v>5.0</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="83">
         <v>0.0</v>
       </c>
@@ -17981,10 +17866,10 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="95">
+      <c r="B14" s="96">
         <v>6.0</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="83">
         <v>0.0</v>
       </c>
@@ -17998,10 +17883,10 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="95">
+      <c r="B15" s="96">
         <v>7.0</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="83">
         <v>0.0</v>
       </c>
@@ -18015,10 +17900,10 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="95">
+      <c r="B16" s="96">
         <v>8.0</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="83">
         <v>0.0</v>
       </c>
@@ -18032,10 +17917,10 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="8"/>
-      <c r="B17" s="95">
+      <c r="B17" s="96">
         <v>9.0</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="83">
         <v>0.0</v>
       </c>
@@ -18049,10 +17934,10 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="8"/>
-      <c r="B18" s="95">
+      <c r="B18" s="96">
         <v>10.0</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="83">
         <v>0.0</v>
       </c>
@@ -18066,10 +17951,10 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="95">
+      <c r="B19" s="96">
         <v>11.0</v>
       </c>
-      <c r="C19" s="82"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="83">
         <v>0.0</v>
       </c>
@@ -18083,10 +17968,10 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="95">
+      <c r="B20" s="96">
         <v>12.0</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="83">
         <v>0.0</v>
       </c>
@@ -18100,10 +17985,10 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="95">
+      <c r="B21" s="96">
         <v>13.0</v>
       </c>
-      <c r="C21" s="82"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="83">
         <v>0.0</v>
       </c>
@@ -18117,10 +18002,10 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="8"/>
-      <c r="B22" s="95">
+      <c r="B22" s="96">
         <v>14.0</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="83">
         <v>0.0</v>
       </c>
@@ -18134,10 +18019,10 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="95">
+      <c r="B23" s="96">
         <v>15.0</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="83">
         <v>0.0</v>
       </c>
@@ -18151,10 +18036,10 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="95">
+      <c r="B24" s="96">
         <v>16.0</v>
       </c>
-      <c r="C24" s="82"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="83">
         <v>0.0</v>
       </c>
@@ -18168,10 +18053,10 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="95">
+      <c r="B25" s="96">
         <v>17.0</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="83">
         <v>0.0</v>
       </c>
@@ -18185,10 +18070,10 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="95">
+      <c r="B26" s="96">
         <v>18.0</v>
       </c>
-      <c r="C26" s="82"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="83">
         <v>0.0</v>
       </c>
@@ -18202,10 +18087,10 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="95">
+      <c r="B27" s="96">
         <v>19.0</v>
       </c>
-      <c r="C27" s="82"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="83">
         <v>0.0</v>
       </c>
@@ -18219,10 +18104,10 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="95">
+      <c r="B28" s="96">
         <v>20.0</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="83">
         <v>0.0</v>
       </c>
@@ -18236,10 +18121,10 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="95">
+      <c r="B29" s="96">
         <v>21.0</v>
       </c>
-      <c r="C29" s="82"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="83">
         <v>0.0</v>
       </c>
@@ -18253,10 +18138,10 @@
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="95">
+      <c r="B30" s="96">
         <v>22.0</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="83">
         <v>0.0</v>
       </c>
@@ -18270,10 +18155,10 @@
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="95">
+      <c r="B31" s="96">
         <v>23.0</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="83">
         <v>0.0</v>
       </c>
@@ -18287,10 +18172,10 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="95">
+      <c r="B32" s="96">
         <v>24.0</v>
       </c>
-      <c r="C32" s="82"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="83">
         <v>0.0</v>
       </c>
@@ -18304,10 +18189,10 @@
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="B33" s="95">
+      <c r="B33" s="96">
         <v>25.0</v>
       </c>
-      <c r="C33" s="82"/>
+      <c r="C33" s="85"/>
       <c r="D33" s="83">
         <v>0.0</v>
       </c>
@@ -18321,10 +18206,10 @@
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="95">
+      <c r="B34" s="96">
         <v>26.0</v>
       </c>
-      <c r="C34" s="82"/>
+      <c r="C34" s="85"/>
       <c r="D34" s="83">
         <v>0.0</v>
       </c>
@@ -18338,10 +18223,10 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="8"/>
-      <c r="B35" s="95">
+      <c r="B35" s="96">
         <v>27.0</v>
       </c>
-      <c r="C35" s="82"/>
+      <c r="C35" s="85"/>
       <c r="D35" s="83">
         <v>0.0</v>
       </c>
@@ -18355,10 +18240,10 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="8"/>
-      <c r="B36" s="95">
+      <c r="B36" s="96">
         <v>28.0</v>
       </c>
-      <c r="C36" s="82"/>
+      <c r="C36" s="85"/>
       <c r="D36" s="83">
         <v>0.0</v>
       </c>
@@ -18372,10 +18257,10 @@
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="8"/>
-      <c r="B37" s="95">
+      <c r="B37" s="96">
         <v>29.0</v>
       </c>
-      <c r="C37" s="82"/>
+      <c r="C37" s="85"/>
       <c r="D37" s="83">
         <v>0.0</v>
       </c>
@@ -18389,10 +18274,10 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="8"/>
-      <c r="B38" s="95">
+      <c r="B38" s="96">
         <v>30.0</v>
       </c>
-      <c r="C38" s="82"/>
+      <c r="C38" s="85"/>
       <c r="D38" s="83">
         <v>0.0</v>
       </c>
@@ -18406,30 +18291,30 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="22"/>
-      <c r="B39" s="99"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="66"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101"/>
+      <c r="D39" s="101"/>
+      <c r="E39" s="102"/>
+      <c r="F39" s="102"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="22"/>
       <c r="B40" s="72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C40" s="72" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
       </c>
-      <c r="D40" s="88">
+      <c r="D40" s="89">
         <f t="shared" ref="D40:F40" si="2">SUM(D9:D38)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="89">
+      <c r="E40" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F40" s="89">
+      <c r="F40" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -18438,7 +18323,7 @@
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="48"/>
-      <c r="D41" s="90"/>
+      <c r="D41" s="91"/>
       <c r="E41" s="8"/>
       <c r="F41" s="62"/>
       <c r="G41" s="8"/>
@@ -18451,7 +18336,7 @@
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="8"/>
       <c r="B42" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C42" s="56"/>
       <c r="D42" s="57"/>
@@ -18467,17 +18352,17 @@
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="8"/>
       <c r="B43" s="58" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D43" s="59"/>
       <c r="E43" s="58" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F43" s="58" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G43" s="60"/>
       <c r="H43" s="62"/>
@@ -18489,68 +18374,68 @@
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="8"/>
       <c r="B44" s="58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D44" s="59"/>
       <c r="E44" s="61" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F44" s="58" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G44" s="60"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="8"/>
       <c r="B45" s="58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D45" s="59"/>
       <c r="E45" s="60" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F45" s="60" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G45" s="60"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="8"/>
       <c r="B46" s="58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C46" s="58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D46" s="60"/>
       <c r="E46" s="58" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F46" s="58" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G46" s="58"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="8"/>
       <c r="B47" s="58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F47" s="61" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G47" s="58"/>
       <c r="H47" s="62"/>
@@ -18562,10 +18447,10 @@
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="8"/>
       <c r="B48" s="58" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D48" s="59"/>
       <c r="E48" s="58"/>
@@ -18579,7 +18464,7 @@
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="8"/>
-      <c r="H49" s="91"/>
+      <c r="H49" s="92"/>
       <c r="I49" s="8"/>
       <c r="J49" s="62"/>
       <c r="K49" s="62"/>
@@ -18588,9 +18473,9 @@
     <row r="50" ht="13.5" customHeight="1">
       <c r="A50" s="8"/>
       <c r="B50" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="H50" s="91"/>
+        <v>67</v>
+      </c>
+      <c r="H50" s="92"/>
       <c r="I50" s="8"/>
       <c r="J50" s="62"/>
       <c r="K50" s="62"/>
@@ -19590,18 +19475,18 @@
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="62"/>
       <c r="E1" s="8"/>
       <c r="F1" s="62"/>
       <c r="G1" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H1" s="63" t="str">
-        <f>Overview!H9</f>
-        <v>Your Name</v>
+        <f>Overview!H5</f>
+        <v>Malhar Prajapati</v>
       </c>
       <c r="K1" s="62"/>
       <c r="L1" s="62"/>
@@ -19617,7 +19502,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="62"/>
       <c r="G2" s="64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" s="65">
         <v>45931.0</v>
@@ -19635,7 +19520,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="62"/>
       <c r="G3" s="64" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="66" t="str">
         <f>Overview!H3</f>
@@ -19662,7 +19547,7 @@
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="70" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>Overview!H4</f>
@@ -19691,19 +19576,19 @@
     <row r="7" ht="33.75" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="72" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
@@ -19722,7 +19607,7 @@
       <c r="B9" s="81">
         <v>1.0</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="84">
         <v>0.0</v>
       </c>
@@ -19739,7 +19624,7 @@
       <c r="B10" s="81">
         <v>2.0</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="83">
         <v>0.0</v>
       </c>
@@ -19756,7 +19641,7 @@
       <c r="B11" s="81">
         <v>3.0</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="83">
         <v>0.0</v>
       </c>
@@ -19773,7 +19658,7 @@
       <c r="B12" s="81">
         <v>4.0</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="83">
         <v>0.0</v>
       </c>
@@ -19790,7 +19675,7 @@
       <c r="B13" s="81">
         <v>5.0</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="83">
         <v>0.0</v>
       </c>
@@ -19807,7 +19692,7 @@
       <c r="B14" s="81">
         <v>6.0</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="83">
         <v>0.0</v>
       </c>
@@ -19824,7 +19709,7 @@
       <c r="B15" s="81">
         <v>7.0</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="83">
         <v>0.0</v>
       </c>
@@ -19841,7 +19726,7 @@
       <c r="B16" s="81">
         <v>8.0</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="83">
         <v>0.0</v>
       </c>
@@ -19858,7 +19743,7 @@
       <c r="B17" s="81">
         <v>9.0</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="83">
         <v>0.0</v>
       </c>
@@ -19875,7 +19760,7 @@
       <c r="B18" s="81">
         <v>10.0</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="83">
         <v>0.0</v>
       </c>
@@ -19892,7 +19777,7 @@
       <c r="B19" s="81">
         <v>11.0</v>
       </c>
-      <c r="C19" s="82"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="83">
         <v>0.0</v>
       </c>
@@ -19909,7 +19794,7 @@
       <c r="B20" s="81">
         <v>12.0</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="83">
         <v>0.0</v>
       </c>
@@ -19926,7 +19811,7 @@
       <c r="B21" s="81">
         <v>13.0</v>
       </c>
-      <c r="C21" s="82"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="83">
         <v>0.0</v>
       </c>
@@ -19943,7 +19828,7 @@
       <c r="B22" s="81">
         <v>14.0</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="83">
         <v>0.0</v>
       </c>
@@ -19960,7 +19845,7 @@
       <c r="B23" s="81">
         <v>15.0</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="83">
         <v>0.0</v>
       </c>
@@ -19977,7 +19862,7 @@
       <c r="B24" s="81">
         <v>16.0</v>
       </c>
-      <c r="C24" s="82"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="83">
         <v>0.0</v>
       </c>
@@ -19994,7 +19879,7 @@
       <c r="B25" s="81">
         <v>17.0</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="83">
         <v>0.0</v>
       </c>
@@ -20011,7 +19896,7 @@
       <c r="B26" s="81">
         <v>18.0</v>
       </c>
-      <c r="C26" s="82"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="83">
         <v>0.0</v>
       </c>
@@ -20028,7 +19913,7 @@
       <c r="B27" s="81">
         <v>19.0</v>
       </c>
-      <c r="C27" s="82"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="83">
         <v>0.0</v>
       </c>
@@ -20045,7 +19930,7 @@
       <c r="B28" s="81">
         <v>20.0</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="83">
         <v>0.0</v>
       </c>
@@ -20062,7 +19947,7 @@
       <c r="B29" s="81">
         <v>21.0</v>
       </c>
-      <c r="C29" s="82"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="83">
         <v>0.0</v>
       </c>
@@ -20079,7 +19964,7 @@
       <c r="B30" s="81">
         <v>22.0</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="83">
         <v>0.0</v>
       </c>
@@ -20096,7 +19981,7 @@
       <c r="B31" s="81">
         <v>23.0</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="83">
         <v>0.0</v>
       </c>
@@ -20113,7 +19998,7 @@
       <c r="B32" s="81">
         <v>24.0</v>
       </c>
-      <c r="C32" s="82"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="83">
         <v>0.0</v>
       </c>
@@ -20130,7 +20015,7 @@
       <c r="B33" s="81">
         <v>25.0</v>
       </c>
-      <c r="C33" s="82"/>
+      <c r="C33" s="85"/>
       <c r="D33" s="83">
         <v>0.0</v>
       </c>
@@ -20147,7 +20032,7 @@
       <c r="B34" s="81">
         <v>26.0</v>
       </c>
-      <c r="C34" s="82"/>
+      <c r="C34" s="85"/>
       <c r="D34" s="83">
         <v>0.0</v>
       </c>
@@ -20164,7 +20049,7 @@
       <c r="B35" s="81">
         <v>27.0</v>
       </c>
-      <c r="C35" s="82"/>
+      <c r="C35" s="85"/>
       <c r="D35" s="83">
         <v>0.0</v>
       </c>
@@ -20181,7 +20066,7 @@
       <c r="B36" s="81">
         <v>28.0</v>
       </c>
-      <c r="C36" s="82"/>
+      <c r="C36" s="85"/>
       <c r="D36" s="83">
         <v>0.0</v>
       </c>
@@ -20198,7 +20083,7 @@
       <c r="B37" s="81">
         <v>29.0</v>
       </c>
-      <c r="C37" s="82"/>
+      <c r="C37" s="85"/>
       <c r="D37" s="83">
         <v>0.0</v>
       </c>
@@ -20215,7 +20100,7 @@
       <c r="B38" s="81">
         <v>30.0</v>
       </c>
-      <c r="C38" s="82"/>
+      <c r="C38" s="85"/>
       <c r="D38" s="83">
         <v>0.0</v>
       </c>
@@ -20232,7 +20117,7 @@
       <c r="B39" s="81">
         <v>31.0</v>
       </c>
-      <c r="C39" s="82"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="83">
         <v>0.0</v>
       </c>
@@ -20246,30 +20131,30 @@
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="8"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="88"/>
       <c r="F40" s="84"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="22"/>
       <c r="B41" s="72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C41" s="72" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
       </c>
-      <c r="D41" s="88">
+      <c r="D41" s="89">
         <f t="shared" ref="D41:F41" si="2">SUM(D9:D40)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="89">
+      <c r="E41" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F41" s="89">
+      <c r="F41" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20278,7 +20163,7 @@
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="48"/>
-      <c r="D42" s="90"/>
+      <c r="D42" s="91"/>
       <c r="E42" s="8"/>
       <c r="F42" s="62"/>
       <c r="G42" s="8"/>
@@ -20291,7 +20176,7 @@
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="8"/>
       <c r="B43" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C43" s="56"/>
       <c r="D43" s="57"/>
@@ -20307,17 +20192,17 @@
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="8"/>
       <c r="B44" s="58" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D44" s="59"/>
       <c r="E44" s="58" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F44" s="58" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G44" s="60"/>
       <c r="H44" s="62"/>
@@ -20329,68 +20214,68 @@
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="8"/>
       <c r="B45" s="58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D45" s="59"/>
       <c r="E45" s="61" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F45" s="58" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G45" s="60"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="8"/>
       <c r="B46" s="58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C46" s="58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="60" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F46" s="60" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G46" s="60"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="8"/>
       <c r="B47" s="58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D47" s="60"/>
       <c r="E47" s="58" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F47" s="58" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G47" s="58"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="8"/>
       <c r="B48" s="58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D48" s="59"/>
       <c r="E48" s="58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F48" s="61" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G48" s="58"/>
       <c r="H48" s="62"/>
@@ -20402,10 +20287,10 @@
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="8"/>
       <c r="B49" s="58" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="58"/>
@@ -20419,7 +20304,7 @@
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="8"/>
-      <c r="H50" s="91"/>
+      <c r="H50" s="92"/>
       <c r="I50" s="8"/>
       <c r="J50" s="62"/>
       <c r="K50" s="62"/>
@@ -20428,9 +20313,9 @@
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="8"/>
       <c r="B51" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="H51" s="91"/>
+        <v>67</v>
+      </c>
+      <c r="H51" s="92"/>
       <c r="I51" s="8"/>
       <c r="J51" s="62"/>
       <c r="K51" s="62"/>
@@ -21429,18 +21314,18 @@
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="62"/>
       <c r="E1" s="8"/>
       <c r="F1" s="62"/>
       <c r="G1" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H1" s="63" t="str">
-        <f>Overview!H9</f>
-        <v>Your Name</v>
+        <f>Overview!H5</f>
+        <v>Malhar Prajapati</v>
       </c>
       <c r="K1" s="62"/>
       <c r="L1" s="62"/>
@@ -21456,7 +21341,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="62"/>
       <c r="G2" s="64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" s="65">
         <v>45962.0</v>
@@ -21474,7 +21359,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="62"/>
       <c r="G3" s="64" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="66" t="str">
         <f>Overview!H3</f>
@@ -21501,7 +21386,7 @@
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="70" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="71" t="str">
         <f>Overview!H4</f>
@@ -21530,24 +21415,24 @@
     <row r="7" ht="33.75" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="72" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="22"/>
-      <c r="B8" s="98"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="77" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
@@ -21558,10 +21443,10 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="8"/>
-      <c r="B9" s="95">
+      <c r="B9" s="96">
         <v>1.0</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="84">
         <v>0.0</v>
       </c>
@@ -21575,10 +21460,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="8"/>
-      <c r="B10" s="95">
+      <c r="B10" s="96">
         <v>2.0</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="83">
         <v>0.0</v>
       </c>
@@ -21592,10 +21477,10 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="8"/>
-      <c r="B11" s="95">
+      <c r="B11" s="96">
         <v>3.0</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="83">
         <v>0.0</v>
       </c>
@@ -21609,10 +21494,10 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="8"/>
-      <c r="B12" s="95">
+      <c r="B12" s="96">
         <v>4.0</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="83">
         <v>0.0</v>
       </c>
@@ -21626,10 +21511,10 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="8"/>
-      <c r="B13" s="95">
+      <c r="B13" s="96">
         <v>5.0</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="83">
         <v>0.0</v>
       </c>
@@ -21643,10 +21528,10 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="95">
+      <c r="B14" s="96">
         <v>6.0</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="83">
         <v>0.0</v>
       </c>
@@ -21660,10 +21545,10 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="95">
+      <c r="B15" s="96">
         <v>7.0</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="83">
         <v>0.0</v>
       </c>
@@ -21677,10 +21562,10 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="95">
+      <c r="B16" s="96">
         <v>8.0</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="83">
         <v>0.0</v>
       </c>
@@ -21694,10 +21579,10 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="8"/>
-      <c r="B17" s="95">
+      <c r="B17" s="96">
         <v>9.0</v>
       </c>
-      <c r="C17" s="82"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="83">
         <v>0.0</v>
       </c>
@@ -21711,10 +21596,10 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="8"/>
-      <c r="B18" s="95">
+      <c r="B18" s="96">
         <v>10.0</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="83">
         <v>0.0</v>
       </c>
@@ -21728,10 +21613,10 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="95">
+      <c r="B19" s="96">
         <v>11.0</v>
       </c>
-      <c r="C19" s="82"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="83">
         <v>0.0</v>
       </c>
@@ -21745,10 +21630,10 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="95">
+      <c r="B20" s="96">
         <v>12.0</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="83">
         <v>0.0</v>
       </c>
@@ -21762,10 +21647,10 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="95">
+      <c r="B21" s="96">
         <v>13.0</v>
       </c>
-      <c r="C21" s="82"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="83">
         <v>0.0</v>
       </c>
@@ -21779,10 +21664,10 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="8"/>
-      <c r="B22" s="95">
+      <c r="B22" s="96">
         <v>14.0</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="83">
         <v>0.0</v>
       </c>
@@ -21796,10 +21681,10 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="95">
+      <c r="B23" s="96">
         <v>15.0</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="83">
         <v>0.0</v>
       </c>
@@ -21813,10 +21698,10 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="95">
+      <c r="B24" s="96">
         <v>16.0</v>
       </c>
-      <c r="C24" s="82"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="83">
         <v>0.0</v>
       </c>
@@ -21830,10 +21715,10 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="95">
+      <c r="B25" s="96">
         <v>17.0</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="83">
         <v>0.0</v>
       </c>
@@ -21847,10 +21732,10 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="95">
+      <c r="B26" s="96">
         <v>18.0</v>
       </c>
-      <c r="C26" s="82"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="83">
         <v>0.0</v>
       </c>
@@ -21864,10 +21749,10 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="95">
+      <c r="B27" s="96">
         <v>19.0</v>
       </c>
-      <c r="C27" s="82"/>
+      <c r="C27" s="85"/>
       <c r="D27" s="83">
         <v>0.0</v>
       </c>
@@ -21881,10 +21766,10 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="95">
+      <c r="B28" s="96">
         <v>20.0</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="83">
         <v>0.0</v>
       </c>
@@ -21898,30 +21783,30 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="22"/>
-      <c r="B29" s="99"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="66"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" s="72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C30" s="72" t="str">
         <f>Overview!H4</f>
         <v>Service-Booking-System</v>
       </c>
-      <c r="D30" s="88">
+      <c r="D30" s="89">
         <f t="shared" ref="D30:F30" si="2">SUM(D9:D28)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="89">
+      <c r="E30" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F30" s="89">
+      <c r="F30" s="90">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -21930,7 +21815,7 @@
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="48"/>
-      <c r="D31" s="90"/>
+      <c r="D31" s="91"/>
       <c r="E31" s="8"/>
       <c r="F31" s="62"/>
       <c r="G31" s="8"/>
@@ -21943,7 +21828,7 @@
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="8"/>
       <c r="B32" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C32" s="56"/>
       <c r="D32" s="57"/>
@@ -21959,17 +21844,17 @@
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="8"/>
       <c r="B33" s="58" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D33" s="59"/>
       <c r="E33" s="58" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F33" s="58" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G33" s="60"/>
       <c r="H33" s="62"/>
@@ -21981,68 +21866,68 @@
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="8"/>
       <c r="B34" s="58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D34" s="59"/>
       <c r="E34" s="61" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F34" s="58" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G34" s="60"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="8"/>
       <c r="B35" s="58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D35" s="59"/>
       <c r="E35" s="60" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F35" s="60" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G35" s="60"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="8"/>
       <c r="B36" s="58" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D36" s="60"/>
       <c r="E36" s="58" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F36" s="58" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G36" s="58"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="8"/>
       <c r="B37" s="58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D37" s="59"/>
       <c r="E37" s="58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F37" s="61" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G37" s="58"/>
       <c r="H37" s="62"/>
@@ -22054,10 +21939,10 @@
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="8"/>
       <c r="B38" s="58" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D38" s="59"/>
       <c r="E38" s="58"/>
@@ -22071,7 +21956,7 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="8"/>
-      <c r="H39" s="91"/>
+      <c r="H39" s="92"/>
       <c r="I39" s="8"/>
       <c r="J39" s="62"/>
       <c r="K39" s="62"/>
@@ -22080,9 +21965,9 @@
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="8"/>
       <c r="B40" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="H40" s="91"/>
+        <v>67</v>
+      </c>
+      <c r="H40" s="92"/>
       <c r="I40" s="8"/>
       <c r="J40" s="62"/>
       <c r="K40" s="62"/>

</xml_diff>